<commit_message>
Added script to generate stock change percentage distribution
</commit_message>
<xml_diff>
--- a/data_distribution_plot.xlsx
+++ b/data_distribution_plot.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,18 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gloriaxiang/Google 云端硬盘/EngSci 2019 Summer/APS360/Project/News_Stock_Prediction_Group/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2026354F-2A3C-154E-B4CE-5C16805FBB99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A902BD2-1891-F148-ABA6-2B2CCE64837E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="1480" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1280" yWindow="1200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="date_distribution" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">date_distribution!$B$1:$B$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">date_distribution!$B$1:$B$11</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">date_distribution!$B$1:$B$11</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,13 +27,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1203,531 +1194,531 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>date_distribution!$B$1:$B$174</c:f>
+              <c:f>date_distribution!$C$1:$C$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="174"/>
                 <c:pt idx="0">
-                  <c:v>396</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>364</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>396</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>380</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>356</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>364</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>518</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>541</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>448</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="110">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>422</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>356</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>383</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>348</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>336</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="111">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>373</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>319</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>378</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>345</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="124">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>516</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>311</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>484</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>474</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>407</c:v>
-                </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="125">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="138">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="139">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="144">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>315</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>415</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>501</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>402</c:v>
-                </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="145">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="158">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>444</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>385</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>467</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>405</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>396</c:v>
-                </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="159">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="41">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>490</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>471</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>358</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>353</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>317</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>381</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>386</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>486</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>317</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>433</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>471</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>479</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>390</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>458</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>434</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>437</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>455</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>458</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>470</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>404</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>421</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>436</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>470</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>502</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>338</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>497</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>508</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>492</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>415</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>542</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>547</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>540</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>521</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>422</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>556</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>583</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>485</c:v>
-                </c:pt>
-                <c:pt idx="97">
+                <c:pt idx="160">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="166">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="98">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>527</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>553</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>539</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>514</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>574</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>421</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>532</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>532</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>441</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>404</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>382</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>471</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>497</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>443</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>549</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>369</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>535</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>383</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>377</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>378</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>542</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>467</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>355</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>371</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>395</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>411</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>444</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>367</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>420</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>471</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>454</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>502</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>356</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>351</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>451</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>374</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>539</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>524</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>310</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>8</c:v>
-                </c:pt>
                 <c:pt idx="167">
-                  <c:v>94</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>106</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>134</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>50</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>63</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>29</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>17</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2571,16 +2562,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>813953</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>156232</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>116026</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>45766</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171621</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171622</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114413</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2904,1405 +2895,2111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B174"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H177" sqref="H177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>43466</v>
       </c>
       <c r="B1">
         <v>396</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <f>ROUND(B1/3,0)</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>43467</v>
       </c>
       <c r="B2">
         <v>364</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f t="shared" ref="C2:C65" si="0">ROUND(B2/3,0)</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>43468</v>
       </c>
       <c r="B3">
         <v>396</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>43469</v>
       </c>
       <c r="B4">
         <v>380</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>43472</v>
       </c>
       <c r="B5">
         <v>356</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>43473</v>
       </c>
       <c r="B6">
         <v>364</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>43474</v>
       </c>
       <c r="B7">
         <v>518</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>43475</v>
       </c>
       <c r="B8">
         <v>541</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>43476</v>
       </c>
       <c r="B9">
         <v>448</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>43477</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>43479</v>
       </c>
       <c r="B11">
         <v>422</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>43480</v>
       </c>
       <c r="B12">
         <v>356</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>43481</v>
       </c>
       <c r="B13">
         <v>383</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>43482</v>
       </c>
       <c r="B14">
         <v>348</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>43483</v>
       </c>
       <c r="B15">
         <v>336</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>43484</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>43486</v>
       </c>
       <c r="B17">
         <v>373</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>43487</v>
       </c>
       <c r="B18">
         <v>319</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>43488</v>
       </c>
       <c r="B19">
         <v>379</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>43489</v>
       </c>
       <c r="B20">
         <v>378</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>43490</v>
       </c>
       <c r="B21">
         <v>345</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>43492</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>43493</v>
       </c>
       <c r="B23">
         <v>516</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>43494</v>
       </c>
       <c r="B24">
         <v>311</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>43495</v>
       </c>
       <c r="B25">
         <v>484</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>43496</v>
       </c>
       <c r="B26">
         <v>474</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>43497</v>
       </c>
       <c r="B27">
         <v>407</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>43498</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>43499</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>43500</v>
       </c>
       <c r="B30">
         <v>318</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>43501</v>
       </c>
       <c r="B31">
         <v>315</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>43502</v>
       </c>
       <c r="B32">
         <v>415</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>43503</v>
       </c>
       <c r="B33">
         <v>501</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>43504</v>
       </c>
       <c r="B34">
         <v>402</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>43505</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>43507</v>
       </c>
       <c r="B36">
         <v>444</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>43508</v>
       </c>
       <c r="B37">
         <v>385</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>43509</v>
       </c>
       <c r="B38">
         <v>467</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>43510</v>
       </c>
       <c r="B39">
         <v>405</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>43511</v>
       </c>
       <c r="B40">
         <v>396</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>43512</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>43513</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>43514</v>
       </c>
       <c r="B43">
         <v>318</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>43515</v>
       </c>
       <c r="B44">
         <v>490</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>43516</v>
       </c>
       <c r="B45">
         <v>471</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>43517</v>
       </c>
       <c r="B46">
         <v>301</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>43518</v>
       </c>
       <c r="B47">
         <v>358</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>43519</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>43520</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>43521</v>
       </c>
       <c r="B50">
         <v>353</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>43522</v>
       </c>
       <c r="B51">
         <v>317</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="1">
         <v>43523</v>
       </c>
       <c r="B52">
         <v>381</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="1">
         <v>43524</v>
       </c>
       <c r="B53">
         <v>386</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="1">
         <v>43525</v>
       </c>
       <c r="B54">
         <v>486</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>43526</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="1">
         <v>43528</v>
       </c>
       <c r="B56">
         <v>317</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="1">
         <v>43529</v>
       </c>
       <c r="B57">
         <v>433</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="1">
         <v>43530</v>
       </c>
       <c r="B58">
         <v>471</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>43531</v>
       </c>
       <c r="B59">
         <v>479</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="1">
         <v>43532</v>
       </c>
       <c r="B60">
         <v>448</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="1">
         <v>43533</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="1">
         <v>43535</v>
       </c>
       <c r="B62">
         <v>390</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" s="1">
         <v>43536</v>
       </c>
       <c r="B63">
         <v>458</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="1">
         <v>43537</v>
       </c>
       <c r="B64">
         <v>434</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
         <v>43538</v>
       </c>
       <c r="B65">
         <v>437</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
         <v>43539</v>
       </c>
       <c r="B66">
         <v>455</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <f t="shared" ref="C66:C129" si="1">ROUND(B66/3,0)</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
         <v>43541</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="1">
         <v>43542</v>
       </c>
       <c r="B68">
         <v>401</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="1">
         <v>43543</v>
       </c>
       <c r="B69">
         <v>458</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="1">
         <v>43544</v>
       </c>
       <c r="B70">
         <v>470</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="1">
         <v>43545</v>
       </c>
       <c r="B71">
         <v>480</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" s="1">
         <v>43546</v>
       </c>
       <c r="B72">
         <v>404</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
         <v>43548</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="1">
         <v>43549</v>
       </c>
       <c r="B74">
         <v>352</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="1">
         <v>43550</v>
       </c>
       <c r="B75">
         <v>421</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="1">
         <v>43551</v>
       </c>
       <c r="B76">
         <v>436</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="1">
         <v>43552</v>
       </c>
       <c r="B77">
         <v>470</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="1">
         <v>43553</v>
       </c>
       <c r="B78">
         <v>502</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" s="1">
         <v>43554</v>
       </c>
       <c r="B79">
         <v>4</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="1">
         <v>43555</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" s="1">
         <v>43556</v>
       </c>
       <c r="B81">
         <v>338</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="1">
         <v>43557</v>
       </c>
       <c r="B82">
         <v>480</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" s="1">
         <v>43558</v>
       </c>
       <c r="B83">
         <v>497</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="1">
         <v>43559</v>
       </c>
       <c r="B84">
         <v>508</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="1">
         <v>43560</v>
       </c>
       <c r="B85">
         <v>492</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="1">
         <v>43561</v>
       </c>
       <c r="B86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="1">
         <v>43563</v>
       </c>
       <c r="B87">
         <v>415</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="1">
         <v>43564</v>
       </c>
       <c r="B88">
         <v>542</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" s="1">
         <v>43565</v>
       </c>
       <c r="B89">
         <v>547</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" s="1">
         <v>43566</v>
       </c>
       <c r="B90">
         <v>540</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" s="1">
         <v>43567</v>
       </c>
       <c r="B91">
         <v>521</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" s="1">
         <v>43568</v>
       </c>
       <c r="B92">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" s="1">
         <v>43569</v>
       </c>
       <c r="B93">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" s="1">
         <v>43570</v>
       </c>
       <c r="B94">
         <v>422</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" s="1">
         <v>43571</v>
       </c>
       <c r="B95">
         <v>556</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" s="1">
         <v>43572</v>
       </c>
       <c r="B96">
         <v>583</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" s="1">
         <v>43574</v>
       </c>
       <c r="B97">
         <v>485</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="1">
         <v>43576</v>
       </c>
       <c r="B98">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" s="1">
         <v>43577</v>
       </c>
       <c r="B99">
         <v>288</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="1">
         <v>43578</v>
       </c>
       <c r="B100">
         <v>527</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="1">
         <v>43579</v>
       </c>
       <c r="B101">
         <v>553</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="1">
         <v>43580</v>
       </c>
       <c r="B102">
         <v>539</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="1">
         <v>43581</v>
       </c>
       <c r="B103">
         <v>514</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="1">
         <v>43582</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="1">
         <v>43583</v>
       </c>
       <c r="B105">
         <v>3</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" s="1">
         <v>43584</v>
       </c>
       <c r="B106">
         <v>459</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="1">
         <v>43585</v>
       </c>
       <c r="B107">
         <v>574</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" s="1">
         <v>43586</v>
       </c>
       <c r="B108">
         <v>421</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" s="1">
         <v>43587</v>
       </c>
       <c r="B109">
         <v>532</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" s="1">
         <v>43588</v>
       </c>
       <c r="B110">
         <v>368</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" s="1">
         <v>43589</v>
       </c>
       <c r="B111">
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" s="1">
         <v>43590</v>
       </c>
       <c r="B112">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" s="1">
         <v>43591</v>
       </c>
       <c r="B113">
         <v>532</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="1">
         <v>43592</v>
       </c>
       <c r="B114">
         <v>380</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" s="1">
         <v>43593</v>
       </c>
       <c r="B115">
         <v>441</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" s="1">
         <v>43594</v>
       </c>
       <c r="B116">
         <v>404</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" s="1">
         <v>43595</v>
       </c>
       <c r="B117">
         <v>382</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="1">
         <v>43596</v>
       </c>
       <c r="B118">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" s="1">
         <v>43598</v>
       </c>
       <c r="B119">
         <v>301</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" s="1">
         <v>43599</v>
       </c>
       <c r="B120">
         <v>471</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" s="1">
         <v>43600</v>
       </c>
       <c r="B121">
         <v>497</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" s="1">
         <v>43601</v>
       </c>
       <c r="B122">
         <v>443</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" s="1">
         <v>43602</v>
       </c>
       <c r="B123">
         <v>549</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" s="1">
         <v>43603</v>
       </c>
       <c r="B124">
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" s="1">
         <v>43604</v>
       </c>
       <c r="B125">
         <v>3</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
       <c r="A126" s="1">
         <v>43605</v>
       </c>
       <c r="B126">
         <v>369</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" s="1">
         <v>43606</v>
       </c>
       <c r="B127">
         <v>535</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" s="1">
         <v>43607</v>
       </c>
       <c r="B128">
         <v>383</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" s="1">
         <v>43608</v>
       </c>
       <c r="B129">
         <v>377</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" s="1">
         <v>43609</v>
       </c>
       <c r="B130">
         <v>378</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C130">
+        <f t="shared" ref="C130:C174" si="2">ROUND(B130/3,0)</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" s="1">
         <v>43610</v>
       </c>
       <c r="B131">
         <v>7</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C131">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" s="1">
         <v>43611</v>
       </c>
       <c r="B132">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C132">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" s="1">
         <v>43612</v>
       </c>
       <c r="B133">
         <v>401</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" s="1">
         <v>43613</v>
       </c>
       <c r="B134">
         <v>542</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" s="1">
         <v>43614</v>
       </c>
       <c r="B135">
         <v>467</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" s="1">
         <v>43615</v>
       </c>
       <c r="B136">
         <v>355</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" s="1">
         <v>43616</v>
       </c>
       <c r="B137">
         <v>371</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" s="1">
         <v>43617</v>
       </c>
       <c r="B138">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" s="1">
         <v>43618</v>
       </c>
       <c r="B139">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
       <c r="A140" s="1">
         <v>43619</v>
       </c>
       <c r="B140">
         <v>340</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
       <c r="A141" s="1">
         <v>43620</v>
       </c>
       <c r="B141">
         <v>395</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
       <c r="A142" s="1">
         <v>43621</v>
       </c>
       <c r="B142">
         <v>411</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" s="1">
         <v>43622</v>
       </c>
       <c r="B143">
         <v>460</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
       <c r="A144" s="1">
         <v>43623</v>
       </c>
       <c r="B144">
         <v>444</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" s="1">
         <v>43624</v>
       </c>
       <c r="B145">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
       <c r="A146" s="1">
         <v>43625</v>
       </c>
       <c r="B146">
         <v>4</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
       <c r="A147" s="1">
         <v>43626</v>
       </c>
       <c r="B147">
         <v>325</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
       <c r="A148" s="1">
         <v>43627</v>
       </c>
       <c r="B148">
         <v>367</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" s="1">
         <v>43628</v>
       </c>
       <c r="B149">
         <v>420</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
       <c r="A150" s="1">
         <v>43629</v>
       </c>
       <c r="B150">
         <v>471</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
       <c r="A151" s="1">
         <v>43630</v>
       </c>
       <c r="B151">
         <v>454</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" s="1">
         <v>43631</v>
       </c>
       <c r="B152">
         <v>3</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
       <c r="A153" s="1">
         <v>43632</v>
       </c>
       <c r="B153">
         <v>11</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
       <c r="A154" s="1">
         <v>43633</v>
       </c>
       <c r="B154">
         <v>502</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
       <c r="A155" s="1">
         <v>43634</v>
       </c>
       <c r="B155">
         <v>356</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
       <c r="A156" s="1">
         <v>43635</v>
       </c>
       <c r="B156">
         <v>351</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
       <c r="A157" s="1">
         <v>43636</v>
       </c>
       <c r="B157">
         <v>451</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
       <c r="A158" s="1">
         <v>43637</v>
       </c>
       <c r="B158">
         <v>320</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
       <c r="A159" s="1">
         <v>43638</v>
       </c>
       <c r="B159">
         <v>7</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
       <c r="A160" s="1">
         <v>43639</v>
       </c>
       <c r="B160">
         <v>7</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
       <c r="A161" s="1">
         <v>43640</v>
       </c>
       <c r="B161">
         <v>374</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C161">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" s="1">
         <v>43641</v>
       </c>
       <c r="B162">
         <v>364</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
       <c r="A163" s="1">
         <v>43642</v>
       </c>
       <c r="B163">
         <v>539</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C163">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
       <c r="A164" s="1">
         <v>43643</v>
       </c>
       <c r="B164">
         <v>524</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C164">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" s="1">
         <v>43644</v>
       </c>
       <c r="B165">
         <v>310</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C165">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" s="1">
         <v>43645</v>
       </c>
       <c r="B166">
         <v>14</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C166">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" s="1">
         <v>43646</v>
       </c>
       <c r="B167">
         <v>8</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C167">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
       <c r="A168" s="1">
         <v>43647</v>
       </c>
       <c r="B168">
         <v>94</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C168">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" s="1">
         <v>43648</v>
       </c>
       <c r="B169">
         <v>106</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C169">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
       <c r="A170" s="1">
         <v>43649</v>
       </c>
       <c r="B170">
         <v>134</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C170">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" s="1">
         <v>43650</v>
       </c>
       <c r="B171">
         <v>50</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C171">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" s="1">
         <v>43651</v>
       </c>
       <c r="B172">
         <v>63</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C172">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
       <c r="A173" s="1">
         <v>43652</v>
       </c>
       <c r="B173">
         <v>29</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C173">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" s="1">
         <v>43653</v>
       </c>
       <c r="B174">
         <v>17</v>
+      </c>
+      <c r="C174">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="B175">
+        <f>SUM(B1:B174)</f>
+        <v>55308</v>
+      </c>
+      <c r="C175">
+        <f>SUM(C1:C174)</f>
+        <v>18435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added updated news+stock data
</commit_message>
<xml_diff>
--- a/data_distribution_plot.xlsx
+++ b/data_distribution_plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gloriaxiang/Google 云端硬盘/EngSci 2019 Summer/APS360/Project/News_Stock_Prediction_Group/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A902BD2-1891-F148-ABA6-2B2CCE64837E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAF2F69-EF82-8143-8626-C33B1EB2F180}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="1200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -601,12 +601,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Data</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Date Range Distribution</a:t>
+              <a:t>Distribution of Dates For News-Stock Data</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2899,7 +2895,7 @@
   <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="H177" sqref="H177"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>